<commit_message>
ajoute de produit, ajout de la lecture des produits
</commit_message>
<xml_diff>
--- a/etat.xlsx
+++ b/etat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darks\Desktop\Projet Final\ProjetSIAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB833D24-0C1E-4BFC-865F-D2215F20D46A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A48C304-C7F0-4CD8-8FC4-961AFC083B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{55FD4BA1-70F5-420B-9A68-5CC4DEB59ED8}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{55FD4BA1-70F5-420B-9A68-5CC4DEB59ED8}"/>
   </bookViews>
   <sheets>
     <sheet name="Fromage" sheetId="1" r:id="rId1"/>
@@ -462,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F0777C-DE11-49FA-9068-4640E2A15889}">
-  <dimension ref="B1:F7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,122 +473,122 @@
     <col min="3" max="4" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>200</v>
+      </c>
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="E2">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>800</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>200</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2">
+      <c r="E4">
         <v>200</v>
       </c>
-      <c r="E2">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>135</v>
+      </c>
+      <c r="D5">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3">
-        <v>800</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4">
+      <c r="E5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>260</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
         <v>200</v>
       </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5">
-        <v>135</v>
-      </c>
-      <c r="E5">
+      <c r="D7">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6">
-        <v>260</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7">
-        <v>200</v>
-      </c>
       <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
         <v>200</v>
       </c>
     </row>
@@ -601,7 +601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB943C98-06E6-4C3C-8347-5E1DD9399155}">
   <dimension ref="B1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
début ampl phase 1
</commit_message>
<xml_diff>
--- a/etat.xlsx
+++ b/etat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamof7\Downloads\git\ProjetSIAD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darks\Desktop\ProjetSIAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFD7BFE-730C-4585-90AD-F67245F0237C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09D02E9-0321-44E8-9921-E7F2EB7D09A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{55FD4BA1-70F5-420B-9A68-5CC4DEB59ED8}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{55FD4BA1-70F5-420B-9A68-5CC4DEB59ED8}"/>
   </bookViews>
   <sheets>
     <sheet name="Fromage" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t># de lot</t>
   </si>
@@ -101,13 +101,31 @@
   </si>
   <si>
     <t>Limite de séchage</t>
+  </si>
+  <si>
+    <t>Gain</t>
+  </si>
+  <si>
+    <t>Brie</t>
+  </si>
+  <si>
+    <t>Dorémi</t>
+  </si>
+  <si>
+    <t>Bleu</t>
+  </si>
+  <si>
+    <t>Sauv</t>
+  </si>
+  <si>
+    <t>Do</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +138,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -480,19 +499,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F0777C-DE11-49FA-9068-4640E2A15889}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.75" customWidth="1"/>
-    <col min="3" max="4" width="19.25" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="4" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,8 +527,11 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -525,8 +547,11 @@
       <c r="E2">
         <v>800</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -542,8 +567,11 @@
       <c r="E3">
         <v>500</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -559,8 +587,11 @@
       <c r="E4">
         <v>200</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -576,8 +607,11 @@
       <c r="E5">
         <v>1000</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -593,8 +627,11 @@
       <c r="E6">
         <v>1200</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -609,6 +646,73 @@
       </c>
       <c r="E7">
         <v>200</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16">
+        <v>30</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <v>30</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -625,13 +729,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.875" customWidth="1"/>
-    <col min="2" max="2" width="20.125" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -639,7 +743,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
formatage des données pour la résolution 1 (problem1)
</commit_message>
<xml_diff>
--- a/etat.xlsx
+++ b/etat.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darks\Desktop\ProjetSIAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6BE879-EC71-42F2-BEA2-1A691A9F3D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D485A6D-D9C0-44F4-A527-47971EC29FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{55FD4BA1-70F5-420B-9A68-5CC4DEB59ED8}"/>
+    <workbookView xWindow="4095" yWindow="1260" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{55FD4BA1-70F5-420B-9A68-5CC4DEB59ED8}"/>
   </bookViews>
   <sheets>
     <sheet name="Fromage" sheetId="1" r:id="rId1"/>
-    <sheet name="Lignes" sheetId="3" r:id="rId2"/>
-    <sheet name="infos" sheetId="2" r:id="rId3"/>
+    <sheet name="infos" sheetId="2" r:id="rId2"/>
+    <sheet name="lignes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t># de lot</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Gain</t>
   </si>
   <si>
-    <t xml:space="preserve">GF </t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -123,6 +120,15 @@
   </si>
   <si>
     <t>Temps journée</t>
+  </si>
+  <si>
+    <t>002-204</t>
+  </si>
+  <si>
+    <t>Chèvre DC</t>
+  </si>
+  <si>
+    <t>nom</t>
   </si>
 </sst>
 </file>
@@ -503,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F0777C-DE11-49FA-9068-4640E2A15889}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,6 +661,26 @@
         <v>3</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>800</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -662,66 +688,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92F3A5F9-8121-4742-8A37-B410E3A62A68}">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="5" width="20.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB943C98-06E6-4C3C-8347-5E1DD9399155}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,7 +710,7 @@
         <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -755,5 +726,110 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92F3A5F9-8121-4742-8A37-B410E3A62A68}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="5" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>